<commit_message>
Update histogram plot for paper to have SciAV strict discard; calculate the flight height in meters
</commit_message>
<xml_diff>
--- a/00_raw_reports/CM_2021_performer_info.xlsx
+++ b/00_raw_reports/CM_2021_performer_info.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13F56C45-03DB-A141-AF3D-4A68B12AB56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F61878-6571-8D43-B6E7-1730B8AC1B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1240" windowWidth="29280" windowHeight="19540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Performer Info" sheetId="6" r:id="rId1"/>
@@ -358,7 +358,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -505,7 +505,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -961,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="84.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>